<commit_message>
Fixing bugs in code, plotting some findings, adding plots
</commit_message>
<xml_diff>
--- a/Data/ReplicationStudiesTrackingDocument.xls.xlsx
+++ b/Data/ReplicationStudiesTrackingDocument.xls.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{250B137E-56D7-422B-9BA0-DAEE41B44565}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDD93D8-AAE4-4439-A5E0-CCC82D209D73}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16200" windowHeight="9015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="9015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
   <si>
     <t>Open Science Collaboration. (2015). Estimating the reproducibility of psychological science. Science, 349(6251), aac4716. Doi: 10.1126/science.aac4716</t>
   </si>
@@ -126,9 +126,6 @@
   </si>
   <si>
     <t xml:space="preserve">Cova, F., Strickland, B., Abatista, A., Allard, A., Andow, J., Attie, M., . . . Colombo, M. (2018). Estimating the reproducibility of experimental philosophy. Review of Philosophy and Psychology, 1-36. </t>
-  </si>
-  <si>
-    <t>In press</t>
   </si>
   <si>
     <t>Explanation_sampling_from_paper</t>
@@ -704,14 +701,14 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
         <v>22</v>
@@ -723,37 +720,37 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F1" t="s">
+        <v>87</v>
+      </c>
+      <c r="G1" t="s">
         <v>88</v>
       </c>
-      <c r="G1" t="s">
-        <v>89</v>
-      </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K1" t="s">
         <v>11</v>
       </c>
       <c r="L1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M1" t="s">
         <v>17</v>
       </c>
       <c r="N1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="O1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
@@ -773,13 +770,13 @@
         <v>0.36</v>
       </c>
       <c r="G2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H2" t="s">
         <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K2">
         <v>100</v>
@@ -788,7 +785,7 @@
         <v>3</v>
       </c>
       <c r="N2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O2">
         <v>1</v>
@@ -796,7 +793,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
         <v>23</v>
@@ -811,14 +808,14 @@
         <v>0.85</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K3">
         <v>13</v>
@@ -829,10 +826,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
+        <v>43</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>103</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
@@ -841,10 +838,10 @@
         <v>0.54</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K4">
         <v>28</v>
@@ -852,7 +849,7 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>25</v>
@@ -865,7 +862,7 @@
         <v>0.3</v>
       </c>
       <c r="G5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H5" t="s">
         <v>21</v>
@@ -874,7 +871,7 @@
         <v>20</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="K5">
         <v>10</v>
@@ -888,7 +885,7 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
@@ -903,7 +900,7 @@
         <v>0.62</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
@@ -912,7 +909,7 @@
         <v>27</v>
       </c>
       <c r="J6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="K6">
         <v>21</v>
@@ -923,7 +920,7 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -935,7 +932,7 @@
         <v>0.61</v>
       </c>
       <c r="G7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H7" t="s">
         <v>30</v>
@@ -944,7 +941,7 @@
         <v>29</v>
       </c>
       <c r="J7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K7">
         <v>18</v>
@@ -955,7 +952,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
         <v>31</v>
@@ -970,10 +967,10 @@
         <v>0.7</v>
       </c>
       <c r="G8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="J8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K8">
         <v>40</v>
@@ -986,17 +983,14 @@
       <c r="A9" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>104</v>
-      </c>
       <c r="E9" s="4">
         <v>0.88</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K9">
         <v>38</v>
@@ -1033,154 +1027,154 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" t="s">
         <v>65</v>
-      </c>
-      <c r="B1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mixture models changing tracked variables, estimates, and saving output modules
</commit_message>
<xml_diff>
--- a/Data/ReplicationStudiesTrackingDocument.xls.xlsx
+++ b/Data/ReplicationStudiesTrackingDocument.xls.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDD93D8-AAE4-4439-A5E0-CCC82D209D73}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CB16B2-8B41-4CE8-AC13-A07B8A9B2B92}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16170" windowHeight="9015" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
     <definedName name="_ftn1" localSheetId="0">Sheet1!#REF!</definedName>
     <definedName name="_ftnref1" localSheetId="0">Sheet1!$J$4</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="106">
   <si>
     <t>Open Science Collaboration. (2015). Estimating the reproducibility of psychological science. Science, 349(6251), aac4716. Doi: 10.1126/science.aac4716</t>
   </si>
@@ -62,9 +63,6 @@
     <t>https://psyarxiv.com/sxdah/</t>
   </si>
   <si>
-    <t>LOOPR</t>
-  </si>
-  <si>
     <t>n_studies</t>
   </si>
   <si>
@@ -83,9 +81,6 @@
     <t>RPPdataConverted.csv</t>
   </si>
   <si>
-    <t>Not_applicable_estimate</t>
-  </si>
-  <si>
     <t>ManyLabs1_Table2.xlsx</t>
   </si>
   <si>
@@ -342,13 +337,25 @@
   </si>
   <si>
     <t>Klein et al. (2018)</t>
+  </si>
+  <si>
+    <t>n_included</t>
+  </si>
+  <si>
+    <t>n_with_sample_size_and_effect_size_rep_and_orig</t>
+  </si>
+  <si>
+    <t>N_dropped_a_priori_applicable_estimate</t>
+  </si>
+  <si>
+    <t>loopr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,13 +391,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFBCBCBC"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -406,7 +431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -417,6 +442,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -698,20 +732,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O9"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="4" width="9.140625" customWidth="1"/>
+    <col min="7" max="10" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
         <v>6</v>
@@ -720,83 +758,106 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" t="s">
         <v>85</v>
       </c>
-      <c r="F1" t="s">
-        <v>87</v>
-      </c>
       <c r="G1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>82</v>
+      </c>
+      <c r="M1" t="s">
+        <v>104</v>
+      </c>
+      <c r="N1" t="s">
+        <v>102</v>
+      </c>
+      <c r="O1" t="s">
+        <v>103</v>
+      </c>
+      <c r="P1" t="s">
         <v>34</v>
       </c>
-      <c r="I1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>84</v>
-      </c>
-      <c r="M1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>36</v>
       </c>
-      <c r="O1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
       </c>
       <c r="E2" s="4">
         <v>0.36</v>
       </c>
+      <c r="F2">
+        <f>ROUND( E2*L2,0)</f>
+        <v>35</v>
+      </c>
       <c r="G2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K2">
         <v>100</v>
       </c>
+      <c r="L2">
+        <v>97</v>
+      </c>
       <c r="M2">
         <v>3</v>
       </c>
-      <c r="N2" t="s">
-        <v>37</v>
+      <c r="N2">
+        <v>95</v>
       </c>
       <c r="O2">
+        <v>90</v>
+      </c>
+      <c r="P2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <f>E2*K2</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -807,29 +868,43 @@
       <c r="E3" s="4">
         <v>0.85</v>
       </c>
+      <c r="F3">
+        <f>ROUND( E3*K3,0)</f>
+        <v>11</v>
+      </c>
       <c r="G3" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K3">
         <v>13</v>
       </c>
+      <c r="N3">
+        <v>16</v>
+      </c>
       <c r="O3">
+        <v>15</v>
+      </c>
+      <c r="Q3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <f>E3*K3</f>
+        <v>11.049999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>2</v>
@@ -837,22 +912,36 @@
       <c r="E4" s="4">
         <v>0.54</v>
       </c>
+      <c r="F4">
+        <f t="shared" ref="F4:F8" si="0">ROUND( E4*K4,0)</f>
+        <v>15</v>
+      </c>
       <c r="G4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K4">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N4">
+        <v>22</v>
+      </c>
+      <c r="O4">
+        <v>22</v>
+      </c>
+      <c r="R4">
+        <f>E4*K4</f>
+        <v>15.120000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
@@ -861,101 +950,143 @@
       <c r="E5" s="4">
         <v>0.3</v>
       </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="G5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K5">
         <v>10</v>
       </c>
-      <c r="N5" t="s">
-        <v>19</v>
+      <c r="N5">
+        <v>9</v>
       </c>
       <c r="O5">
+        <v>6</v>
+      </c>
+      <c r="P5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <f>E5*K5</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
       </c>
       <c r="E6" s="4">
         <v>0.62</v>
       </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
       <c r="G6" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K6">
         <v>21</v>
       </c>
+      <c r="N6">
+        <v>21</v>
+      </c>
       <c r="O6">
+        <v>21</v>
+      </c>
+      <c r="Q6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <f>E6*K6</f>
+        <v>13.02</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" s="4">
         <v>0.61</v>
       </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
       <c r="G7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="J7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K7">
         <v>18</v>
       </c>
+      <c r="N7">
+        <v>18</v>
+      </c>
       <c r="O7">
+        <v>18</v>
+      </c>
+      <c r="Q7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <f>E7*K7</f>
+        <v>10.98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>
@@ -966,41 +1097,115 @@
       <c r="E8" s="4">
         <v>0.7</v>
       </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
       <c r="G8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K8">
         <v>40</v>
       </c>
+      <c r="N8">
+        <v>40</v>
+      </c>
       <c r="O8">
+        <v>33</v>
+      </c>
+      <c r="Q8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <f>E8*K8</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>105</v>
       </c>
       <c r="E9" s="4">
         <v>0.88</v>
       </c>
+      <c r="F9">
+        <f>ROUND( E9*K9,0)</f>
+        <v>69</v>
+      </c>
       <c r="G9" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K9">
-        <v>38</v>
-      </c>
-      <c r="L9">
         <v>78</v>
       </c>
+      <c r="N9">
+        <v>121</v>
+      </c>
       <c r="O9">
+        <v>100</v>
+      </c>
+      <c r="Q9">
         <v>1</v>
       </c>
+      <c r="R9">
+        <f>E9*N9</f>
+        <v>106.48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <f>SUM(R2:R9)/SUM(K2:K8,N9)</f>
+        <v>0.63717948717948725</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="E12" s="4"/>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D18" s="1"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D20" s="7"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E21" s="4"/>
+      <c r="K21" s="8"/>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E22" s="4"/>
+      <c r="K22" s="9"/>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E23" s="4"/>
+      <c r="K23" s="9"/>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E24" s="4"/>
+      <c r="K24" s="9"/>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="E25" s="4"/>
+      <c r="K25" s="9"/>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="9"/>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K27" s="9"/>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="K28" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1027,154 +1232,154 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B14" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>